<commit_message>
พัฒนา Extend The Repayment Report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_extend_the_repayment.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_extend_the_repayment.xlsx
@@ -229,21 +229,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -342,130 +350,130 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="10.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="162.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="131.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="29.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="6.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="24.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="61.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="37.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+    <row r="2" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="W2" s="9" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>